<commit_message>
modify practise stim schedule
</commit_message>
<xml_diff>
--- a/clock-practise/clock_types_practise.xlsx
+++ b/clock-practise/clock_types_practise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jocel\Documents\Collab project Marco Pang\clock-practise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UBSN PC8\Downloads\collab-main\clock-practise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BD91EA-96E4-4A1D-B15F-08DE7132986B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAEF821-0DD4-4429-BC6C-3C7341DF69D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trialTypes" sheetId="1" r:id="rId1"/>
@@ -365,16 +365,16 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="1" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -405,7 +405,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>

</xml_diff>